<commit_message>
Acho que entendi essa bagaça
</commit_message>
<xml_diff>
--- a/Perceptron_RU_Uninter.xlsx
+++ b/Perceptron_RU_Uninter.xlsx
@@ -1,22 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e16b601b2ec7f0ec/Ambiente de Trabalho/Perceptron_uninter/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="1" documentId="11_7B16B235F726F496FA6C78BC7CB2A5F9AC2F1D32" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{02EFD85B-867F-4301-9690-1A6D7FC3E58F}"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="105" windowWidth="14355" windowHeight="4695"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
     <sheet name="Plan2" sheetId="2" r:id="rId2"/>
     <sheet name="Plan3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>X1</t>
   </si>
@@ -60,17 +77,32 @@
     <t>W7</t>
   </si>
   <si>
-    <t>Resultado perceptron</t>
-  </si>
-  <si>
-    <t>taxa de aprendizagem</t>
+    <t>Saída esperada</t>
+  </si>
+  <si>
+    <t>Bias</t>
+  </si>
+  <si>
+    <t>Taxa aprendizado</t>
+  </si>
+  <si>
+    <t>W bias</t>
+  </si>
+  <si>
+    <t>Novos valores dos pesos</t>
+  </si>
+  <si>
+    <t>ERRO</t>
+  </si>
+  <si>
+    <t>Saída Perceptron</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -82,6 +114,12 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -107,14 +145,25 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -126,14 +175,17 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Escritório">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -171,7 +223,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Escritório">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -243,7 +295,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Escritório">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -416,140 +468,383 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:M17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="7.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.85546875" customWidth="1"/>
-    <col min="2" max="2" width="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15" customWidth="1"/>
+    <col min="12" max="12" width="12" customWidth="1"/>
+    <col min="13" max="13" width="9.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" s="4"/>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
+      <c r="K1" s="4"/>
+      <c r="L1" s="4"/>
+      <c r="M1" s="6"/>
+    </row>
+    <row r="2" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="4"/>
+      <c r="B2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="I2" s="4"/>
+      <c r="J2" s="4" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
+      <c r="K2" s="4"/>
+      <c r="L2" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="M2" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" s="4"/>
+      <c r="B3" s="4">
+        <v>4</v>
+      </c>
+      <c r="C3" s="4">
+        <v>7</v>
+      </c>
+      <c r="D3" s="4">
+        <v>4</v>
+      </c>
+      <c r="E3" s="4">
+        <v>2</v>
+      </c>
+      <c r="F3" s="4">
         <v>0</v>
       </c>
-      <c r="B2" s="1">
+      <c r="G3" s="4">
+        <v>5</v>
+      </c>
+      <c r="H3" s="4">
+        <v>1</v>
+      </c>
+      <c r="I3" s="4"/>
+      <c r="J3" s="4">
+        <v>1</v>
+      </c>
+      <c r="K3" s="4"/>
+      <c r="L3" s="5">
+        <v>0.1</v>
+      </c>
+      <c r="M3" s="4">
+        <f>M6 - L6</f>
         <v>0</v>
       </c>
-      <c r="C2" s="1">
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" s="4"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
+      <c r="J4" s="4"/>
+      <c r="K4" s="4"/>
+      <c r="L4" s="5"/>
+      <c r="M4" s="4"/>
+    </row>
+    <row r="5" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="4"/>
+      <c r="B5" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="I5" s="4"/>
+      <c r="J5" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="K5" s="4"/>
+      <c r="L5" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="M5" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" s="4"/>
+      <c r="B6" s="4">
+        <v>0.03</v>
+      </c>
+      <c r="C6" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="D6" s="4">
+        <v>0.03</v>
+      </c>
+      <c r="E6" s="4">
+        <v>0.01</v>
+      </c>
+      <c r="F6" s="4">
         <v>0</v>
       </c>
-      <c r="D2" s="1">
+      <c r="G6" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="H6" s="4">
+        <v>0.02</v>
+      </c>
+      <c r="I6" s="4"/>
+      <c r="J6" s="4">
+        <v>0.13</v>
+      </c>
+      <c r="K6" s="4"/>
+      <c r="L6" s="4">
+        <f>IF(SUMPRODUCT(B3:H3, B6:H6) + J3*J6 &gt; 0, 1, 0)</f>
+        <v>1</v>
+      </c>
+      <c r="M6" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" s="2"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
+      <c r="L7" s="1"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" s="1"/>
+      <c r="B8" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+      <c r="K8" s="1"/>
+      <c r="L8" s="1"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1">
+        <f>B6 + ($L$3 * $M$3 * B3)</f>
+        <v>0.03</v>
+      </c>
+      <c r="C9" s="1">
+        <f t="shared" ref="C9:H9" si="0">C6 + ($L$3 * $M$3 * C3)</f>
+        <v>0.5</v>
+      </c>
+      <c r="D9" s="1">
+        <f t="shared" si="0"/>
+        <v>0.03</v>
+      </c>
+      <c r="E9" s="1">
+        <f t="shared" si="0"/>
+        <v>0.01</v>
+      </c>
+      <c r="F9" s="1">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E2" s="1">
-        <v>0</v>
-      </c>
-      <c r="F2" s="1">
-        <v>0</v>
-      </c>
-      <c r="G2" s="1">
-        <v>0</v>
-      </c>
-      <c r="I2" s="1">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
-        <v>0.03</v>
-      </c>
-      <c r="B5" s="1">
+      <c r="G9" s="1">
+        <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
-      <c r="C5" s="1">
-        <v>0.03</v>
-      </c>
-      <c r="D5" s="1">
-        <v>0.01</v>
-      </c>
-      <c r="E5" s="1">
-        <v>0</v>
-      </c>
-      <c r="F5" s="1">
-        <v>0.5</v>
-      </c>
-      <c r="G5" s="1">
+      <c r="H9" s="1">
+        <f t="shared" si="0"/>
         <v>0.02</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="2">
-        <f>IF(SUMPRODUCT(A$2:G$2,A$5:G$5) * I2 &gt; 0, 1, 0)</f>
-        <v>0</v>
-      </c>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1">
+        <f>J6 + ($L$3 * $M$3 * J3)</f>
+        <v>0.13</v>
+      </c>
+      <c r="K9" s="1"/>
+      <c r="L9" s="1"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+      <c r="K10" s="1"/>
+      <c r="L10" s="1"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
+      <c r="K11" s="1"/>
+      <c r="L11" s="1"/>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
+      <c r="K12" s="1"/>
+      <c r="L12" s="1"/>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
+      <c r="K13" s="1"/>
+      <c r="L13" s="1"/>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="1"/>
+      <c r="K14" s="1"/>
+      <c r="L14" s="1"/>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+      <c r="J15" s="1"/>
+      <c r="K15" s="1"/>
+      <c r="L15" s="1"/>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A16" s="1"/>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
+      <c r="J16" s="1"/>
+      <c r="K16" s="1"/>
+      <c r="L16" s="1"/>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A17" s="1"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+      <c r="I17" s="1"/>
+      <c r="J17" s="1"/>
+      <c r="K17" s="1"/>
+      <c r="L17" s="1"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B8:H8"/>
+  </mergeCells>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -561,7 +856,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>